<commit_message>
Remove rows with all values = NaN from dataframes
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_trimestral.xlsx
+++ b/etl/data/input/Datos_carga_trimestral.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Indice confianza empresarial" sheetId="1" state="visible" r:id="rId2"/>
@@ -239,7 +239,7 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -567,7 +567,7 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -842,7 +842,7 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1117,7 +1117,7 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1392,7 +1392,7 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated quarterly data file
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_trimestral.xlsx
+++ b/etl/data/input/Datos_carga_trimestral.xlsx
@@ -2098,7 +2098,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2367,7 +2367,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add datasets 'Pensiones contributivas' and 'Pensiones no contributivas'
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_trimestral.xlsx
+++ b/etl/data/input/Datos_carga_trimestral.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Indice confianza empresarial" sheetId="1" state="visible" r:id="rId2"/>
@@ -526,7 +526,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="G2:G10 A12"/>
+      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -836,10 +836,31 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="A12" s="1" t="n">
+        <f aca="false">A11</f>
+        <v>2020</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>104.6</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>-27.9614325068871</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>-13.2426206574766</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>95.5</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>-29.2592592592593</v>
+      </c>
+      <c r="H12" s="3" t="n">
+        <v>-13.5336193158822</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="3"/>
@@ -1203,7 +1224,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="G2:G10 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1849,7 +1870,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K25" activeCellId="1" sqref="G2:G10 K25"/>
+      <selection pane="topLeft" activeCell="K25" activeCellId="0" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2503,7 +2524,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="1" sqref="G2:G10 E19"/>
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3151,7 +3172,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F39" activeCellId="1" sqref="G2:G10 F39"/>
+      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3799,7 +3820,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H38" activeCellId="1" sqref="G2:G10 H38"/>
+      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4093,8 +4114,8 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2:G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4327,7 +4348,7 @@
   <dimension ref="A1:H65536"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H25" activeCellId="1" sqref="G2:G10 H25"/>
+      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4977,7 +4998,7 @@
   <dimension ref="A1:H65536"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I33" activeCellId="1" sqref="G2:G10 I33"/>
+      <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5607,7 +5628,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="G2:G10 E1"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5858,7 +5879,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="G2:G10 C1"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5892,7 +5913,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>2018</v>
       </c>
@@ -5902,11 +5923,17 @@
       <c r="C2" s="6" t="n">
         <v>3.13093389161548</v>
       </c>
+      <c r="D2" s="6" t="n">
+        <v>3.13093389161548</v>
+      </c>
       <c r="F2" s="7" t="n">
         <v>-2.68728526121591</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G2" s="7" t="n">
+        <v>-2.68728526121591</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2018</v>
       </c>
@@ -5916,11 +5943,17 @@
       <c r="C3" s="6" t="n">
         <v>3.9869762754208</v>
       </c>
+      <c r="D3" s="6" t="n">
+        <v>3.9869762754208</v>
+      </c>
       <c r="F3" s="7" t="n">
         <v>-2.30188604522251</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="7" t="n">
+        <v>-2.30188604522251</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>2018</v>
       </c>
@@ -5930,11 +5963,17 @@
       <c r="C4" s="6" t="n">
         <v>3.31263894862715</v>
       </c>
+      <c r="D4" s="6" t="n">
+        <v>3.31263894862715</v>
+      </c>
       <c r="F4" s="7" t="n">
         <v>-3.2591826348422</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="7" t="n">
+        <v>-3.2591826348422</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>2018</v>
       </c>
@@ -5944,11 +5983,17 @@
       <c r="C5" s="6" t="n">
         <v>3.41119195971466</v>
       </c>
+      <c r="D5" s="6" t="n">
+        <v>3.41119195971466</v>
+      </c>
       <c r="F5" s="7" t="n">
         <v>-3.1831816498342</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="7" t="n">
+        <v>-3.1831816498342</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>2019</v>
       </c>
@@ -5958,11 +6003,17 @@
       <c r="C6" s="6" t="n">
         <v>5.0758553168718</v>
       </c>
+      <c r="D6" s="6" t="n">
+        <v>5.0758553168718</v>
+      </c>
       <c r="F6" s="7" t="n">
         <v>-3.07890249330125</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="7" t="n">
+        <v>-3.07890249330125</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>2019</v>
       </c>
@@ -5972,11 +6023,17 @@
       <c r="C7" s="6" t="n">
         <v>4.61894894226243</v>
       </c>
+      <c r="D7" s="6" t="n">
+        <v>4.61894894226243</v>
+      </c>
       <c r="F7" s="7" t="n">
         <v>-1.69093659677032</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="7" t="n">
+        <v>-1.69093659677032</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>2019</v>
       </c>
@@ -5986,11 +6043,17 @@
       <c r="C8" s="6" t="n">
         <v>1.46885260047616</v>
       </c>
+      <c r="D8" s="6" t="n">
+        <v>1.46885260047616</v>
+      </c>
       <c r="F8" s="7" t="n">
         <v>-3.44165937673543</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="7" t="n">
+        <v>-3.44165937673543</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>2019</v>
       </c>
@@ -6000,11 +6063,17 @@
       <c r="C9" s="6" t="n">
         <v>1.31996650249306</v>
       </c>
+      <c r="D9" s="6" t="n">
+        <v>1.31996650249306</v>
+      </c>
       <c r="F9" s="7" t="n">
         <v>-2.06959942148175</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="7" t="n">
+        <v>-2.06959942148175</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>2020</v>
       </c>
@@ -6014,7 +6083,13 @@
       <c r="C10" s="6" t="n">
         <v>5.28804313976996</v>
       </c>
+      <c r="D10" s="6" t="n">
+        <v>5.28804313976996</v>
+      </c>
       <c r="F10" s="7" t="n">
+        <v>-2.5565146958697</v>
+      </c>
+      <c r="G10" s="7" t="n">
         <v>-2.5565146958697</v>
       </c>
     </row>
@@ -6037,7 +6112,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="G2:G10 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6681,7 +6756,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="G2:G10 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7325,7 +7400,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="G2:G10 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7969,7 +8044,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="G2:G10 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8613,7 +8688,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="G2:G10 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9257,7 +9332,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E43" activeCellId="1" sqref="G2:G10 E43"/>
+      <selection pane="topLeft" activeCell="E43" activeCellId="0" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9917,7 +9992,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="1" sqref="G2:G10 G19"/>
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10576,8 +10651,8 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="G2:G10 A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fixed errors in quarterly #8937
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_trimestral.xlsx
+++ b/etl/data/input/Datos_carga_trimestral.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\economia\1. Publicaciones\Panel indicadores economicos\envio_informatica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sp-fs-200.ad2.cantabria.es\G2R00001\datos\publicaciones\Panel indicadores socioeconomicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" firstSheet="5" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100"/>
   </bookViews>
   <sheets>
     <sheet name="PIB" sheetId="33" r:id="rId1"/>
@@ -676,8 +676,8 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <f t="shared" ref="A24:A25" si="0">A23</f>
+        <f t="shared" ref="A24" si="0">A23</f>
         <v>2023</v>
       </c>
       <c r="B24" s="1">
@@ -1334,60 +1334,40 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="2">
-        <v>0.62290000000000001</v>
-      </c>
-      <c r="H25" s="2">
-        <v>1.057725596203319</v>
-      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C26" s="5"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="2">
-        <v>0</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0</v>
-      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C27" s="5"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="2">
-        <v>0</v>
-      </c>
-      <c r="H27" s="2">
-        <v>0</v>
-      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C28" s="5"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="2">
-        <v>0</v>
-      </c>
-      <c r="H28" s="2">
-        <v>0</v>
-      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C29" s="5"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="2">
-        <v>0</v>
-      </c>
-      <c r="H29" s="2">
-        <v>0</v>
-      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D30" s="2"/>
@@ -9803,7 +9783,7 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -11185,7 +11165,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:F29"/>
+      <selection activeCell="G23" sqref="B1:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -11842,60 +11822,40 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="2">
-        <v>0</v>
-      </c>
-      <c r="H25" s="2">
-        <v>0</v>
-      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C26" s="3"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="2">
-        <v>0</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0</v>
-      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C27" s="3"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="2">
-        <v>0</v>
-      </c>
-      <c r="H27" s="2">
-        <v>0</v>
-      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C28" s="3"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="2">
-        <v>0</v>
-      </c>
-      <c r="H28" s="2">
-        <v>0</v>
-      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C29" s="3"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="2">
-        <v>0</v>
-      </c>
-      <c r="H29" s="2">
-        <v>0</v>
-      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="str">

</xml_diff>

<commit_message>
Actualiza trimestre panel #9458
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_trimestral.xlsx
+++ b/etl/data/input/Datos_carga_trimestral.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" tabRatio="820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" tabRatio="820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PIB" sheetId="33" r:id="rId1"/>
@@ -677,7 +677,7 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26:E26"/>
     </sheetView>
   </sheetViews>
@@ -11361,8 +11361,8 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -12042,12 +12042,30 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="3"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="A26" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3">
+        <v>3311528</v>
+      </c>
+      <c r="D26" s="2">
+        <v>-1.888791448413174</v>
+      </c>
+      <c r="E26" s="2">
+        <v>-1.9581144840203564</v>
+      </c>
+      <c r="F26" s="3">
+        <v>328932123</v>
+      </c>
+      <c r="G26" s="2">
+        <v>2.0242538370377039</v>
+      </c>
+      <c r="H26" s="2">
+        <v>2.3571880913558845</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C27" s="3"/>
@@ -13220,7 +13238,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <f t="shared" ref="A25:A28" si="0">A24</f>
+        <f t="shared" ref="A25" si="0">A24</f>
         <v>2023</v>
       </c>
       <c r="B25" s="1">

</xml_diff>

<commit_message>
Modifica panel trimestre #9516
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_trimestral.xlsx
+++ b/etl/data/input/Datos_carga_trimestral.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\economia\1. Publicaciones\Panel indicadores economicos\envio_informatica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sp-fs-200.ad2.cantabria.es\G2R00001\datos\publicaciones\Panel indicadores socioeconomicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" tabRatio="820" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" tabRatio="820"/>
   </bookViews>
   <sheets>
     <sheet name="PIB" sheetId="33" r:id="rId1"/>
@@ -677,8 +677,8 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27:H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -1358,12 +1358,6 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>2024</v>
-      </c>
-      <c r="B26" s="1">
-        <v>1</v>
-      </c>
       <c r="C26" s="5"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1378,13 +1372,6 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <f>A26</f>
-        <v>2024</v>
-      </c>
-      <c r="B27" s="1">
-        <v>2</v>
-      </c>
       <c r="C27" s="5"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1393,13 +1380,6 @@
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <f>A27</f>
-        <v>2024</v>
-      </c>
-      <c r="B28" s="1">
-        <v>3</v>
-      </c>
       <c r="C28" s="5"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1408,13 +1388,6 @@
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <f>A28</f>
-        <v>2024</v>
-      </c>
-      <c r="B29" s="1">
-        <v>4</v>
-      </c>
       <c r="C29" s="5"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -2296,7 +2269,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="str">
-        <f t="shared" ref="A30:A54" si="0">IF(C32="","",A31)</f>
+        <f t="shared" ref="A32:A54" si="0">IF(C32="","",A31)</f>
         <v/>
       </c>
       <c r="B32" s="1" t="s">
@@ -3668,7 +3641,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="str">
-        <f t="shared" ref="A30:A54" si="0">IF(C32="","",A31)</f>
+        <f t="shared" ref="A32:A54" si="0">IF(C32="","",A31)</f>
         <v/>
       </c>
       <c r="B32" s="1" t="s">
@@ -5036,7 +5009,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="str">
-        <f t="shared" ref="A30:A54" si="0">IF(C31="","",A30)</f>
+        <f t="shared" ref="A31:A54" si="0">IF(C31="","",A30)</f>
         <v/>
       </c>
       <c r="B31" s="1" t="s">
@@ -6436,7 +6409,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="str">
-        <f t="shared" ref="A30:A54" si="0">IF(C32="","",A31)</f>
+        <f t="shared" ref="A32:A54" si="0">IF(C32="","",A31)</f>
         <v/>
       </c>
       <c r="B32" s="1" t="s">
@@ -7809,7 +7782,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="str">
-        <f t="shared" ref="A30:A54" si="0">IF(C32="","",A31)</f>
+        <f t="shared" ref="A32:A54" si="0">IF(C32="","",A31)</f>
         <v/>
       </c>
       <c r="B32" s="1" t="s">
@@ -9187,7 +9160,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="str">
-        <f t="shared" ref="A30:A52" si="3">IF(C33="","",A32)</f>
+        <f t="shared" ref="A33:A52" si="3">IF(C33="","",A32)</f>
         <v/>
       </c>
       <c r="B33" s="1" t="s">
@@ -9737,7 +9710,7 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A27" sqref="A27:I32"/>
     </sheetView>
   </sheetViews>
@@ -10484,7 +10457,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="str">
-        <f t="shared" ref="A30:A54" si="0">IF(C33="","",A32)</f>
+        <f t="shared" ref="A33:A54" si="0">IF(C33="","",A32)</f>
         <v/>
       </c>
       <c r="B33" s="1" t="s">
@@ -11825,7 +11798,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="str">
-        <f t="shared" ref="A30:A54" si="0">IF(C31="","",A30)</f>
+        <f t="shared" ref="A31:A54" si="0">IF(C31="","",A30)</f>
         <v/>
       </c>
       <c r="B31" s="1" t="s">
@@ -12943,7 +12916,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <f t="shared" ref="A25:A28" si="0">A24</f>
+        <f t="shared" ref="A25" si="0">A24</f>
         <v>2023</v>
       </c>
       <c r="B25" s="1">
@@ -13009,7 +12982,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="str">
-        <f t="shared" ref="A30:A54" si="1">IF(C31="","",A30)</f>
+        <f t="shared" ref="A31:A54" si="1">IF(C31="","",A30)</f>
         <v/>
       </c>
       <c r="B31" s="1" t="s">
@@ -14409,7 +14382,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="str">
-        <f t="shared" ref="A30:A54" si="0">IF(C32="","",A31)</f>
+        <f t="shared" ref="A32:A54" si="0">IF(C32="","",A31)</f>
         <v/>
       </c>
       <c r="B32" s="1" t="s">
@@ -15783,7 +15756,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="str">
-        <f t="shared" ref="A30:A54" si="0">IF(C32="","",A31)</f>
+        <f t="shared" ref="A32:A54" si="0">IF(C32="","",A31)</f>
         <v/>
       </c>
       <c r="B32" s="1" t="s">
@@ -17151,7 +17124,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="str">
-        <f t="shared" ref="A30:A54" si="0">IF(C31="","",A30)</f>
+        <f t="shared" ref="A31:A54" si="0">IF(C31="","",A30)</f>
         <v/>
       </c>
       <c r="B31" s="1" t="s">
@@ -18546,7 +18519,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="str">
-        <f t="shared" ref="A30:A54" si="0">IF(C31="","",A30)</f>
+        <f t="shared" ref="A31:A54" si="0">IF(C31="","",A30)</f>
         <v/>
       </c>
       <c r="B31" s="1" t="s">
@@ -19948,7 +19921,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="str">
-        <f t="shared" ref="A31:A54" si="0">IF(C32="","",A31)</f>
+        <f t="shared" ref="A32:A54" si="0">IF(C32="","",A31)</f>
         <v/>
       </c>
       <c r="B32" s="1" t="s">
@@ -21335,7 +21308,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="str">
-        <f t="shared" ref="A30:A54" si="1">IF(C31="","",A30)</f>
+        <f t="shared" ref="A31:A54" si="1">IF(C31="","",A30)</f>
         <v/>
       </c>
       <c r="B31" s="1" t="s">

</xml_diff>

<commit_message>
Actualización datos trimestrales 10/03/2025
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_trimestral.xlsx
+++ b/etl/data/input/Datos_carga_trimestral.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\economia\1. Publicaciones\Panel indicadores economicos\envio_informatica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sp-fs-200.ad2.cantabria.es\G2R00001\datos\publicaciones\Panel indicadores socioeconomicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" tabRatio="820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" tabRatio="820" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="PIB" sheetId="33" r:id="rId1"/>
@@ -677,7 +677,7 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -5259,7 +5259,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <f t="shared" ref="A28:A29" si="0">A27</f>
+        <f t="shared" ref="A28" si="0">A27</f>
         <v>2024</v>
       </c>
       <c r="B28" s="1">
@@ -6714,7 +6714,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <f t="shared" ref="A28:A29" si="0">A27</f>
+        <f t="shared" ref="A28" si="0">A27</f>
         <v>2024</v>
       </c>
       <c r="B28" s="1">
@@ -12472,7 +12472,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <f t="shared" ref="A27:A29" si="0">A26</f>
+        <f t="shared" ref="A27:A28" si="0">A26</f>
         <v>2024</v>
       </c>
       <c r="B27" s="1">
@@ -20339,8 +20339,8 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -21126,30 +21126,12 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>2025</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1</v>
-      </c>
-      <c r="C30" s="2">
-        <v>0</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0</v>
-      </c>
-      <c r="F30" s="2">
-        <v>0</v>
-      </c>
-      <c r="G30" s="2">
-        <v>0</v>
-      </c>
-      <c r="H30" s="2">
-        <v>0</v>
-      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="str">

</xml_diff>

<commit_message>
Actualización 31/03/2025 - 2
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_trimestral.xlsx
+++ b/etl/data/input/Datos_carga_trimestral.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" tabRatio="820" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" tabRatio="820" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="PIB" sheetId="33" r:id="rId1"/>
@@ -342,9 +342,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -381,13 +380,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -689,29 +687,29 @@
     <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1438,10 +1436,10 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="5"/>
+      <c r="C29" s="4"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="5"/>
+      <c r="F29" s="4"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
@@ -1595,29 +1593,29 @@
     <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="54" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3074,29 +3072,29 @@
     <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>68</v>
       </c>
     </row>
@@ -3107,22 +3105,22 @@
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>41106</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>-13.5556864064603</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>1.0883772921897019</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>13717834</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>6.0207827362256383</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <v>38.020858787799028</v>
       </c>
     </row>
@@ -3134,22 +3132,22 @@
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>106743</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>9.0895154779302878</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>2.0315075005606715</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>23420732</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>-0.40603894750588232</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
         <v>46.421055368823687</v>
       </c>
     </row>
@@ -3161,22 +3159,22 @@
       <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>180029</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>-13.820900809474345</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>3.3013109794072011</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>29128315</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>-2.1503905493510223</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>55.862935907444097</v>
       </c>
     </row>
@@ -3188,22 +3186,22 @@
       <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>53301</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>-11.443951552609278</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>4.9324524264878082</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>16541531</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>5.7302201158246024</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <v>66.340539278634566</v>
       </c>
     </row>
@@ -3214,22 +3212,22 @@
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>44018</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>7.0841239721695093</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>6.9488951571929594</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>14225722</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>3.7023920831816381</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>77.811646028333911</v>
       </c>
     </row>
@@ -3241,22 +3239,22 @@
       <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>87028</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>-18.469595195937906</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>9.364367234426183</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>23899130</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>2.0426261655698941</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>90.196155253004207</v>
       </c>
     </row>
@@ -3268,22 +3266,22 @@
       <c r="B8" s="1">
         <v>3</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>195932</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>8.8335768126246208</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>12.19268123910037</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>28836788</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>-1.0008371579337871</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>103.36764776539182</v>
       </c>
     </row>
@@ -3295,22 +3293,22 @@
       <c r="B9" s="1">
         <v>4</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>65539</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>22.960169602821701</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>15.430253525609434</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>16547511</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>3.6151429997621776E-2</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <v>117.14460842256346</v>
       </c>
     </row>
@@ -3321,22 +3319,22 @@
       <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>19505.209346095799</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>-55.688106351729296</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>19.071401008080741</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>10557630</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>-25.78492676856753</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <v>131.28029177850877</v>
       </c>
     </row>
@@ -3348,22 +3346,22 @@
       <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>0</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>0</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>23.115146798189919</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>204272</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>-99.145274325885495</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>145.45475960159703</v>
       </c>
     </row>
@@ -3375,22 +3373,22 @@
       <c r="B12" s="1">
         <v>3</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>67392</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>-65.604393360961964</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>27.513789315512714</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>6044625</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <v>-79.038494162387295</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <v>159.24990789860561</v>
       </c>
     </row>
@@ -3402,22 +3400,22 @@
       <c r="B13" s="1">
         <v>4</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>17313</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>-73.583667739819035</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>32.205180012876006</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>2126576</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <v>-87.148665439775201</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <v>172.0947576551072</v>
       </c>
     </row>
@@ -3428,22 +3426,22 @@
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>5548.6834651546005</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>-71.552812550226562</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>37.068971478933875</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <v>1214374</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="6">
         <v>-88.497664722101462</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="6">
         <v>183.26939960538641</v>
       </c>
     </row>
@@ -3455,22 +3453,22 @@
       <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>24865</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>0</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>41.918698272494971</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>4208726</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <v>1960.3538419362419</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="6">
         <v>191.89189734429354</v>
       </c>
     </row>
@@ -3482,22 +3480,22 @@
       <c r="B16" s="1">
         <v>3</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>83119</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>23.336597815764492</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>46.500006337349717</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>14299445</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <v>136.56463386893316</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="6">
         <v>196.91046005147416</v>
       </c>
     </row>
@@ -3509,22 +3507,22 @@
       <c r="B17" s="1">
         <v>4</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>46428</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>168.16842834863976</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>50.532342430868226</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>11458258</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <v>438.81253244652436</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="6">
         <v>198.37858562194384</v>
       </c>
     </row>
@@ -3535,22 +3533,22 @@
       <c r="B18" s="1">
         <v>1</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>31131</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="6">
         <v>461.05200802137682</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>53.720676180094621</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <v>9720263</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <v>700.43405079489514</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="6">
         <v>196.31205580935412</v>
       </c>
     </row>
@@ -3562,22 +3560,22 @@
       <c r="B19" s="1">
         <v>2</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>75390</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>203.19726523225418</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>55.843499765771632</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>20592825</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <v>389.28880140926259</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="6">
         <v>190.87692358412187</v>
       </c>
     </row>
@@ -3589,22 +3587,22 @@
       <c r="B20" s="1">
         <v>3</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <v>154391</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
         <v>85.746941132593022</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>56.933887451042793</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>25707266</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="6">
         <v>79.778068309644183</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="6">
         <v>182.55431816352996</v>
       </c>
     </row>
@@ -3616,22 +3614,22 @@
       <c r="B21" s="1">
         <v>4</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>62785</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>35.230895149478769</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>57.117009602468173</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>15638928</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="6">
         <v>36.486087152165702</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="6">
         <v>171.94937618850193</v>
       </c>
     </row>
@@ -3642,22 +3640,22 @@
       <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>57443.522755329803</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="6">
         <v>84.521932335388541</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
         <v>56.536044745158826</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="6">
         <v>13703001</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="6">
         <v>40.973562135098618</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="6">
         <v>159.60299914380261</v>
       </c>
     </row>
@@ -3669,22 +3667,22 @@
       <c r="B23" s="1">
         <v>2</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
         <v>107210.5339906578</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>42.207897586759245</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <v>55.320492582692694</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <v>23835938</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="6">
         <v>15.748752296006007</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="6">
         <v>145.97142395854911</v>
       </c>
     </row>
@@ -3696,22 +3694,22 @@
       <c r="B24" s="1">
         <v>3</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <v>202121.64731923791</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="6">
         <v>30.915433748882968</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>53.617343998391618</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <v>29098504</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="6">
         <v>13.191748978673967</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="6">
         <v>131.43674416372812</v>
       </c>
     </row>
@@ -3723,22 +3721,22 @@
       <c r="B25" s="1">
         <v>4</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6">
         <v>67334.354247006209</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="6">
         <v>7.2459253754976638</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="6">
         <v>51.565394503704979</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="6">
         <v>18531605</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="6">
         <v>18.496645038585768</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="6">
         <v>116.29966412053723</v>
       </c>
     </row>
@@ -3749,22 +3747,22 @@
       <c r="B26" s="1">
         <v>1</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>54221.959873424596</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="6">
         <v>-5.6082265282142663</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
         <v>49.289250916176215</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="6">
         <v>16124998</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="6">
         <v>17.674938504346606</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="6">
         <v>100.78698506818337</v>
       </c>
     </row>
@@ -3776,22 +3774,22 @@
       <c r="B27" s="1">
         <v>2</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
         <v>126423.88040502541</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>17.921136756992407</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <v>46.885820385143639</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="6">
         <v>26400990</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="6">
         <v>10.761279879147189</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="6">
         <v>85.064381358947273</v>
       </c>
     </row>
@@ -3803,22 +3801,22 @@
       <c r="B28" s="1">
         <v>3</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6">
         <v>213327.86064779223</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="6">
         <v>5.5442915081999278</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="6">
         <v>44.417699136542822</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="6">
         <v>31377058</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="6">
         <v>7.8304850311204932</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="6">
         <v>69.245582316007287</v>
       </c>
     </row>
@@ -3830,22 +3828,22 @@
       <c r="B29" s="1">
         <v>4</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <v>73807.549279918196</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="6">
         <v>9.6135102286212248</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="6">
         <v>41.929380469041746</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="6">
         <v>19856459</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="6">
         <v>7.1491595034536948</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="6">
         <v>53.39787782411689</v>
       </c>
     </row>
@@ -4537,7 +4535,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H28"/>
+      <selection activeCell="C2" sqref="C2:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -4548,29 +4546,29 @@
     <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="64.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="64.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4582,13 +4580,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>1751024</v>
+        <v>1751023</v>
       </c>
       <c r="D2" s="2">
-        <v>-7.1182218714228256</v>
+        <v>-7.1182749156861398</v>
       </c>
       <c r="E2" s="2">
-        <v>7.4370916395410385</v>
+        <v>6.8445720675537718</v>
       </c>
       <c r="F2" s="2">
         <v>125529721</v>
@@ -4615,7 +4613,7 @@
         <v>-7.3458449474307912</v>
       </c>
       <c r="E3" s="2">
-        <v>6.9956187106243384</v>
+        <v>6.460127002696054</v>
       </c>
       <c r="F3" s="2">
         <v>156459570</v>
@@ -4642,7 +4640,7 @@
         <v>-11.876513963965362</v>
       </c>
       <c r="E4" s="2">
-        <v>6.7780873232777106</v>
+        <v>6.3192505579219258</v>
       </c>
       <c r="F4" s="2">
         <v>385672944</v>
@@ -4663,13 +4661,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="2">
-        <v>2135362</v>
+        <v>2135363</v>
       </c>
       <c r="D5" s="2">
-        <v>-6.5687036778562469</v>
+        <v>-6.5686599235437182</v>
       </c>
       <c r="E5" s="2">
-        <v>6.8101886385026651</v>
+        <v>6.4517871910827571</v>
       </c>
       <c r="F5" s="2">
         <v>128477002</v>
@@ -4692,10 +4690,10 @@
         <v>1829535</v>
       </c>
       <c r="D6" s="2">
-        <v>4.4837192408556437</v>
+        <v>4.4837789109566151</v>
       </c>
       <c r="E6" s="2">
-        <v>7.1059546914961853</v>
+        <v>6.8762090072037365</v>
       </c>
       <c r="F6" s="2">
         <v>129153915</v>
@@ -4722,7 +4720,7 @@
         <v>-1.0598550947872432</v>
       </c>
       <c r="E7" s="2">
-        <v>7.6710557097575283</v>
+        <v>7.6028503318634106</v>
       </c>
       <c r="F7" s="2">
         <v>158627230</v>
@@ -4749,7 +4747,7 @@
         <v>-14.154263673382294</v>
       </c>
       <c r="E8" s="2">
-        <v>8.5095230236293009</v>
+        <v>8.6405502218301713</v>
       </c>
       <c r="F8" s="2">
         <v>378888595</v>
@@ -4773,10 +4771,10 @@
         <v>1873698</v>
       </c>
       <c r="D9" s="2">
-        <v>-12.253847357028924</v>
+        <v>-12.253888448942874</v>
       </c>
       <c r="E9" s="2">
-        <v>9.6199311442012707</v>
+        <v>9.9927335429807549</v>
       </c>
       <c r="F9" s="2">
         <v>127238397</v>
@@ -4802,7 +4800,7 @@
         <v>-34.860333363395611</v>
       </c>
       <c r="E10" s="2">
-        <v>10.986689715877572</v>
+        <v>11.64857840250739</v>
       </c>
       <c r="F10" s="2">
         <v>100295749</v>
@@ -4823,13 +4821,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="2">
-        <v>605612</v>
+        <v>533031</v>
       </c>
       <c r="D11" s="2">
-        <v>-82.377033795791235</v>
+        <v>-84.489099788650819</v>
       </c>
       <c r="E11" s="2">
-        <v>12.580537271499074</v>
+        <v>13.583358768857353</v>
       </c>
       <c r="F11" s="2">
         <v>37014146</v>
@@ -4856,7 +4854,7 @@
         <v>3.1017421856958993</v>
       </c>
       <c r="E12" s="2">
-        <v>14.343557954482092</v>
+        <v>15.74328054062423</v>
       </c>
       <c r="F12" s="2">
         <v>293170232</v>
@@ -4877,13 +4875,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="2">
-        <v>630824</v>
+        <v>630825</v>
       </c>
       <c r="D13" s="2">
-        <v>-66.332674742674641</v>
+        <v>-66.332621372280911</v>
       </c>
       <c r="E13" s="2">
-        <v>16.158487426325888</v>
+        <v>18.013254329803161</v>
       </c>
       <c r="F13" s="2">
         <v>62929097</v>
@@ -4909,7 +4907,7 @@
         <v>-38.222685405448956</v>
       </c>
       <c r="E14" s="2">
-        <v>17.901035213674227</v>
+        <v>20.270289786917452</v>
       </c>
       <c r="F14" s="2">
         <v>51693146</v>
@@ -4933,10 +4931,10 @@
         <v>1960269</v>
       </c>
       <c r="D15" s="2">
-        <v>223.6839758789456</v>
+        <v>267.75891083257824</v>
       </c>
       <c r="E15" s="2">
-        <v>19.395353866815253</v>
+        <v>22.338680390176609</v>
       </c>
       <c r="F15" s="2">
         <v>96645786</v>
@@ -4963,7 +4961,7 @@
         <v>7.663877600065816</v>
       </c>
       <c r="E16" s="2">
-        <v>20.430518610650157</v>
+        <v>24.006161508294912</v>
       </c>
       <c r="F16" s="2">
         <v>359950312</v>
@@ -4987,10 +4985,10 @@
         <v>1953365</v>
       </c>
       <c r="D17" s="2">
-        <v>209.65293013582234</v>
+        <v>209.65243926604052</v>
       </c>
       <c r="E17" s="2">
-        <v>20.923285058837713</v>
+        <v>25.21385615401314</v>
       </c>
       <c r="F17" s="2">
         <v>117883145</v>
@@ -5016,7 +5014,7 @@
         <v>70.834369010897376</v>
       </c>
       <c r="E18" s="2">
-        <v>20.782429674405076</v>
+        <v>25.892673412629424</v>
       </c>
       <c r="F18" s="2">
         <v>102560633</v>
@@ -5043,7 +5041,7 @@
         <v>32.984503657406194</v>
       </c>
       <c r="E19" s="2">
-        <v>20.034684948552524</v>
+        <v>26.088796483886927</v>
       </c>
       <c r="F19" s="2">
         <v>149802200</v>
@@ -5070,7 +5068,7 @@
         <v>-10.300181388801832</v>
       </c>
       <c r="E20" s="2">
-        <v>18.738065834565639</v>
+        <v>25.876497127277723</v>
       </c>
       <c r="F20" s="2">
         <v>367155879</v>
@@ -5097,7 +5095,7 @@
         <v>-4.4702858912696763</v>
       </c>
       <c r="E21" s="2">
-        <v>16.958680922423039</v>
+        <v>25.334356919277337</v>
       </c>
       <c r="F21" s="2">
         <v>126303148</v>
@@ -5123,7 +5121,7 @@
         <v>-4.1229539673970468</v>
       </c>
       <c r="E22" s="2">
-        <v>14.744489897588744</v>
+        <v>24.518347012288746</v>
       </c>
       <c r="F22" s="2">
         <v>117734683</v>
@@ -5150,7 +5148,7 @@
         <v>33.340033619067277</v>
       </c>
       <c r="E23" s="2">
-        <v>12.130059341268209</v>
+        <v>23.46581065695834</v>
       </c>
       <c r="F23" s="2">
         <v>159467479</v>
@@ -5177,7 +5175,7 @@
         <v>22.698349870259872</v>
       </c>
       <c r="E24" s="2">
-        <v>9.1381636822512764</v>
+        <v>22.196190290820198</v>
       </c>
       <c r="F24" s="2">
         <v>383216515</v>
@@ -5204,7 +5202,7 @@
         <v>41.756035763358199</v>
       </c>
       <c r="E25" s="2">
-        <v>5.8048335832514129</v>
+        <v>20.735099740759722</v>
       </c>
       <c r="F25" s="2">
         <v>141664497</v>
@@ -5224,13 +5222,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="2">
-        <v>1912310.9432079997</v>
+        <v>1912311</v>
       </c>
       <c r="D26" s="2">
-        <v>58.58179800262544</v>
+        <v>58.581802712203412</v>
       </c>
       <c r="E26" s="2">
-        <v>2.1745748233495883</v>
+        <v>19.10846668339946</v>
       </c>
       <c r="F26" s="2">
         <v>142177115</v>
@@ -5251,13 +5249,13 @@
         <v>2</v>
       </c>
       <c r="C27" s="2">
-        <v>2656632.5068739997</v>
+        <v>2656633</v>
       </c>
       <c r="D27" s="2">
-        <v>-23.571697568052763</v>
+        <v>-23.571683381377341</v>
       </c>
       <c r="E27" s="2">
-        <v>-1.685637317010658</v>
+        <v>17.355356880376089</v>
       </c>
       <c r="F27" s="2">
         <v>147146989</v>
@@ -5271,20 +5269,20 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <f t="shared" ref="A28" si="0">A27</f>
+        <f t="shared" ref="A28:A29" si="0">A27</f>
         <v>2024</v>
       </c>
       <c r="B28" s="2">
         <v>3</v>
       </c>
       <c r="C28" s="2">
-        <v>1688375</v>
+        <v>10339088</v>
       </c>
       <c r="D28" s="2">
-        <v>-84.679059474151103</v>
+        <v>-6.1792834296184544</v>
       </c>
       <c r="E28" s="2">
-        <v>-5.6735730428987399</v>
+        <v>15.539506928344288</v>
       </c>
       <c r="F28" s="2">
         <v>60413605</v>
@@ -5297,12 +5295,31 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="3"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="A29" s="1">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="B29" s="2">
+        <v>4</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1967161</v>
+      </c>
+      <c r="D29" s="2">
+        <v>-25.633650003969411</v>
+      </c>
+      <c r="E29" s="2">
+        <v>13.699074023795134</v>
+      </c>
+      <c r="F29" s="2">
+        <v>38369207</v>
+      </c>
+      <c r="G29" s="2">
+        <v>-72.915439074336319</v>
+      </c>
+      <c r="H29" s="2">
+        <v>-17.830190741816459</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="str">
@@ -5992,7 +6009,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H28"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -6003,29 +6020,29 @@
     <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="54" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>80</v>
       </c>
     </row>
@@ -6037,22 +6054,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>1751024</v>
+        <v>80590.98</v>
       </c>
       <c r="D2" s="2">
-        <v>-7.1182218714228256</v>
+        <v>11.200035102301676</v>
       </c>
       <c r="E2" s="2">
-        <v>7.4370916395410385</v>
+        <v>11.976254174239921</v>
       </c>
       <c r="F2" s="2">
-        <v>125529721</v>
+        <v>7965303.0300000003</v>
       </c>
       <c r="G2" s="2">
-        <v>9.1727100979684728</v>
+        <v>11.266686970679274</v>
       </c>
       <c r="H2" s="2">
-        <v>2.4024059610912896</v>
+        <v>7.7477246390322625</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6064,22 +6081,22 @@
         <v>2</v>
       </c>
       <c r="C3" s="2">
-        <v>3473305</v>
+        <v>173533.86</v>
       </c>
       <c r="D3" s="2">
-        <v>-7.3458449474307912</v>
+        <v>1.9144969721443639</v>
       </c>
       <c r="E3" s="2">
-        <v>6.9956187106243384</v>
+        <v>12.263501575091444</v>
       </c>
       <c r="F3" s="2">
-        <v>156459570</v>
+        <v>11097516.369999999</v>
       </c>
       <c r="G3" s="2">
-        <v>-0.42320698845422777</v>
+        <v>8.1434501674888295</v>
       </c>
       <c r="H3" s="2">
-        <v>2.6212525736626291</v>
+        <v>8.9755608890407572</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -6091,22 +6108,22 @@
         <v>3</v>
       </c>
       <c r="C4" s="2">
-        <v>10507477</v>
+        <v>406595.88</v>
       </c>
       <c r="D4" s="2">
-        <v>-11.876513963965362</v>
+        <v>-3.9400477762533526</v>
       </c>
       <c r="E4" s="2">
-        <v>6.7780873232777106</v>
+        <v>12.858892428541814</v>
       </c>
       <c r="F4" s="2">
-        <v>385672944</v>
+        <v>18941756.390000001</v>
       </c>
       <c r="G4" s="2">
-        <v>-3.8516507337941319</v>
+        <v>3.9781532031210487</v>
       </c>
       <c r="H4" s="2">
-        <v>2.9312481488812745</v>
+        <v>10.408545556650795</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6118,22 +6135,22 @@
         <v>4</v>
       </c>
       <c r="C5" s="2">
-        <v>2135362</v>
+        <v>102948.7</v>
       </c>
       <c r="D5" s="2">
-        <v>-6.5687036778562469</v>
+        <v>-1.7504670848456305</v>
       </c>
       <c r="E5" s="2">
-        <v>6.8101886385026651</v>
+        <v>13.788131147767251</v>
       </c>
       <c r="F5" s="2">
-        <v>128477002</v>
+        <v>8938381.8200000003</v>
       </c>
       <c r="G5" s="2">
-        <v>-0.18786917919737522</v>
+        <v>3.9941556524567989</v>
       </c>
       <c r="H5" s="2">
-        <v>3.345720087059366</v>
+        <v>12.074003097470372</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6144,22 +6161,22 @@
         <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>1829535</v>
+        <v>82903.25</v>
       </c>
       <c r="D6" s="2">
-        <v>4.4837192408556437</v>
+        <v>2.8691424276017008</v>
       </c>
       <c r="E6" s="2">
-        <v>7.1059546914961853</v>
+        <v>15.066422808315973</v>
       </c>
       <c r="F6" s="2">
-        <v>129153915</v>
+        <v>8317465.4100000001</v>
       </c>
       <c r="G6" s="2">
-        <v>2.8871202541747021</v>
+        <v>4.4212050523833035</v>
       </c>
       <c r="H6" s="2">
-        <v>3.8737564767073711</v>
+        <v>13.995238971886529</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -6171,22 +6188,22 @@
         <v>2</v>
       </c>
       <c r="C7" s="2">
-        <v>3436493</v>
+        <v>183948.78</v>
       </c>
       <c r="D7" s="2">
-        <v>-1.0598550947872432</v>
+        <v>6.0016644590283441</v>
       </c>
       <c r="E7" s="2">
-        <v>7.6710557097575283</v>
+        <v>16.69926086184082</v>
       </c>
       <c r="F7" s="2">
-        <v>158627230</v>
+        <v>11429924.810000001</v>
       </c>
       <c r="G7" s="2">
-        <v>1.3854441757701341</v>
+        <v>2.9953408394927328</v>
       </c>
       <c r="H7" s="2">
-        <v>4.5222369130443463</v>
+        <v>16.19050873563317</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -6198,22 +6215,22 @@
         <v>3</v>
       </c>
       <c r="C8" s="2">
-        <v>9020221</v>
+        <v>375481.66</v>
       </c>
       <c r="D8" s="2">
-        <v>-14.154263673382294</v>
+        <v>-7.6523697190438948</v>
       </c>
       <c r="E8" s="2">
-        <v>8.5095230236293009</v>
+        <v>18.684515459756678</v>
       </c>
       <c r="F8" s="2">
-        <v>378888595</v>
+        <v>19296877.260000002</v>
       </c>
       <c r="G8" s="2">
-        <v>-1.7590938398831524</v>
+        <v>1.874804335396707</v>
       </c>
       <c r="H8" s="2">
-        <v>5.297424343650265</v>
+        <v>18.67208417324451</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6225,22 +6242,22 @@
         <v>4</v>
       </c>
       <c r="C9" s="2">
-        <v>1873698</v>
+        <v>101355.15</v>
       </c>
       <c r="D9" s="2">
-        <v>-12.253847357028924</v>
+        <v>-1.5479068701207521</v>
       </c>
       <c r="E9" s="2">
-        <v>9.6199311442012707</v>
+        <v>21.013370755726683</v>
       </c>
       <c r="F9" s="2">
-        <v>127238397</v>
+        <v>9021576.2200000007</v>
       </c>
       <c r="G9" s="2">
-        <v>-0.96406748345513327</v>
+        <v>0.93075460050104919</v>
       </c>
       <c r="H9" s="2">
-        <v>6.2036212206443055</v>
+        <v>21.443990089319676</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -6251,22 +6268,22 @@
         <v>1</v>
       </c>
       <c r="C10" s="2">
-        <v>1191753</v>
+        <v>56222.92</v>
       </c>
       <c r="D10" s="2">
-        <v>-34.860333363395611</v>
+        <v>-32.182489830012692</v>
       </c>
       <c r="E10" s="2">
-        <v>10.986689715877572</v>
+        <v>23.660550350177218</v>
       </c>
       <c r="F10" s="2">
-        <v>100295749</v>
+        <v>6440847.5199999996</v>
       </c>
       <c r="G10" s="2">
-        <v>-22.344011793990138</v>
+        <v>-22.562376847924881</v>
       </c>
       <c r="H10" s="2">
-        <v>7.240719672280937</v>
+        <v>24.499752988559145</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -6278,22 +6295,22 @@
         <v>2</v>
       </c>
       <c r="C11" s="2">
-        <v>605612</v>
+        <v>21659.33</v>
       </c>
       <c r="D11" s="2">
-        <v>-82.377033795791235</v>
+        <v>-88.225347295045935</v>
       </c>
       <c r="E11" s="2">
-        <v>12.580537271499074</v>
+        <v>26.586677045018508</v>
       </c>
       <c r="F11" s="2">
-        <v>37014146</v>
+        <v>1261489.28</v>
       </c>
       <c r="G11" s="2">
-        <v>-76.665957036506285</v>
+        <v>-88.96327577853944</v>
       </c>
       <c r="H11" s="2">
-        <v>8.4041320213745667</v>
+        <v>27.820078603482877</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -6305,22 +6322,22 @@
         <v>3</v>
       </c>
       <c r="C12" s="2">
-        <v>9300005</v>
+        <v>407764.87</v>
       </c>
       <c r="D12" s="2">
-        <v>3.1017421856958993</v>
+        <v>8.5978127400417002</v>
       </c>
       <c r="E12" s="2">
-        <v>14.343557954482092</v>
+        <v>29.717471742048161</v>
       </c>
       <c r="F12" s="2">
-        <v>293170232</v>
+        <v>10782999.890000001</v>
       </c>
       <c r="G12" s="2">
-        <v>-22.623632416277928</v>
+        <v>-44.120492944463074</v>
       </c>
       <c r="H12" s="2">
-        <v>9.6707801335731816</v>
+        <v>31.356258835463031</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -6332,22 +6349,22 @@
         <v>4</v>
       </c>
       <c r="C13" s="2">
-        <v>630824</v>
+        <v>28614.880000000001</v>
       </c>
       <c r="D13" s="2">
-        <v>-66.332674742674641</v>
+        <v>-71.767709879567036</v>
       </c>
       <c r="E13" s="2">
-        <v>16.158487426325888</v>
+        <v>32.906897827851239</v>
       </c>
       <c r="F13" s="2">
-        <v>62929097</v>
+        <v>2649720.09</v>
       </c>
       <c r="G13" s="2">
-        <v>-50.54236890456896</v>
+        <v>-70.629078274306266</v>
       </c>
       <c r="H13" s="2">
-        <v>10.964417068863591</v>
+        <v>34.986595989382991</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -6358,22 +6375,22 @@
         <v>1</v>
       </c>
       <c r="C14" s="2">
-        <v>736233</v>
+        <v>35577.57</v>
       </c>
       <c r="D14" s="2">
-        <v>-38.222685405448956</v>
+        <v>-36.720522519997175</v>
       </c>
       <c r="E14" s="2">
-        <v>17.901035213674227</v>
+        <v>35.995718902136545</v>
       </c>
       <c r="F14" s="2">
-        <v>51693146</v>
+        <v>2259815.7599999998</v>
       </c>
       <c r="G14" s="2">
-        <v>-48.459285148765375</v>
+        <v>-64.914310531605324</v>
       </c>
       <c r="H14" s="2">
-        <v>12.188611879388947</v>
+        <v>38.54221940026369</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -6385,22 +6402,22 @@
         <v>2</v>
       </c>
       <c r="C15" s="2">
-        <v>1960269</v>
+        <v>95817.01</v>
       </c>
       <c r="D15" s="2">
-        <v>223.6839758789456</v>
+        <v>342.38215124844578</v>
       </c>
       <c r="E15" s="2">
-        <v>19.395353866815253</v>
+        <v>38.75927693479575</v>
       </c>
       <c r="F15" s="2">
-        <v>96645786</v>
+        <v>5403894.9100000001</v>
       </c>
       <c r="G15" s="2">
-        <v>161.10500023423478</v>
+        <v>328.37422367949091</v>
       </c>
       <c r="H15" s="2">
-        <v>13.208491876059007</v>
+        <v>41.788248606711257</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -6412,22 +6429,22 @@
         <v>3</v>
       </c>
       <c r="C16" s="2">
-        <v>10012746</v>
+        <v>410693.19</v>
       </c>
       <c r="D16" s="2">
-        <v>7.663877600065816</v>
+        <v>0.71813935320126365</v>
       </c>
       <c r="E16" s="2">
-        <v>20.430518610650157</v>
+        <v>40.927466244831685</v>
       </c>
       <c r="F16" s="2">
-        <v>359950312</v>
+        <v>16718291.619999999</v>
       </c>
       <c r="G16" s="2">
-        <v>22.778601887520409</v>
+        <v>55.043047301746739</v>
       </c>
       <c r="H16" s="2">
-        <v>13.851279434140931</v>
+        <v>44.425142816124399</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -6439,22 +6456,22 @@
         <v>4</v>
       </c>
       <c r="C17" s="2">
-        <v>1953365</v>
+        <v>117192.73</v>
       </c>
       <c r="D17" s="2">
-        <v>209.65293013582234</v>
+        <v>309.55170876131575</v>
       </c>
       <c r="E17" s="2">
-        <v>20.923285058837713</v>
+        <v>42.419945447693216</v>
       </c>
       <c r="F17" s="2">
-        <v>117883145</v>
+        <v>8138682.8600000003</v>
       </c>
       <c r="G17" s="2">
-        <v>87.326929226395862</v>
+        <v>207.15255134741426</v>
       </c>
       <c r="H17" s="2">
-        <v>14.036632246625738</v>
+        <v>46.33247747032231</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -6465,22 +6482,22 @@
         <v>1</v>
       </c>
       <c r="C18" s="2">
-        <v>1257739</v>
+        <v>77533.600000000006</v>
       </c>
       <c r="D18" s="2">
-        <v>70.834369010897376</v>
+        <v>117.92831831966039</v>
       </c>
       <c r="E18" s="2">
-        <v>20.782429674405076</v>
+        <v>43.131242329521939</v>
       </c>
       <c r="F18" s="2">
-        <v>102560633</v>
+        <v>7045248.0599999996</v>
       </c>
       <c r="G18" s="2">
-        <v>98.402768908667298</v>
+        <v>211.76205532790871</v>
       </c>
       <c r="H18" s="2">
-        <v>13.689787583037811</v>
+        <v>47.396464201427698</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -6492,22 +6509,22 @@
         <v>2</v>
       </c>
       <c r="C19" s="2">
-        <v>2606854</v>
+        <v>151349.45000000001</v>
       </c>
       <c r="D19" s="2">
-        <v>32.984503657406194</v>
+        <v>57.956765714146186</v>
       </c>
       <c r="E19" s="2">
-        <v>20.034684948552524</v>
+        <v>43.122842028530478</v>
       </c>
       <c r="F19" s="2">
-        <v>149802200</v>
+        <v>11657125.26</v>
       </c>
       <c r="G19" s="2">
-        <v>55.001274447703288</v>
+        <v>115.71709765170097</v>
       </c>
       <c r="H19" s="2">
-        <v>12.781789148513893</v>
+        <v>47.603827187736471</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -6519,22 +6536,22 @@
         <v>3</v>
       </c>
       <c r="C20" s="2">
-        <v>8981415</v>
+        <v>444466.27</v>
       </c>
       <c r="D20" s="2">
-        <v>-10.300181388801832</v>
+        <v>8.2234331667393903</v>
       </c>
       <c r="E20" s="2">
-        <v>18.738065834565639</v>
+        <v>42.502977855425293</v>
       </c>
       <c r="F20" s="2">
-        <v>367155879</v>
+        <v>21026463.140000001</v>
       </c>
       <c r="G20" s="2">
-        <v>2.0018226849043641</v>
+        <v>25.769209067068545</v>
       </c>
       <c r="H20" s="2">
-        <v>11.336626261519243</v>
+        <v>47.044019101998579</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -6546,22 +6563,22 @@
         <v>4</v>
       </c>
       <c r="C21" s="2">
-        <v>1866044</v>
+        <v>110633.95999999999</v>
       </c>
       <c r="D21" s="2">
-        <v>-4.4702858912696763</v>
+        <v>-5.5965672955993089</v>
       </c>
       <c r="E21" s="2">
-        <v>16.958680922423039</v>
+        <v>41.389154323216353</v>
       </c>
       <c r="F21" s="2">
-        <v>126303148</v>
+        <v>10563173.24</v>
       </c>
       <c r="G21" s="2">
-        <v>7.14266912373267</v>
+        <v>29.789714401035148</v>
       </c>
       <c r="H21" s="2">
-        <v>9.4046754188311148</v>
+        <v>45.849063411003954</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -6572,22 +6589,22 @@
         <v>1</v>
       </c>
       <c r="C22" s="2">
-        <v>1205883</v>
+        <v>79721.41</v>
       </c>
       <c r="D22" s="2">
-        <v>-4.1229539673970468</v>
+        <v>2.8217572768451271</v>
       </c>
       <c r="E22" s="2">
-        <v>14.744489897588744</v>
+        <v>39.877451229483199</v>
       </c>
       <c r="F22" s="2">
-        <v>117734683</v>
+        <v>9311544.7400000002</v>
       </c>
       <c r="G22" s="2">
-        <v>14.795199245698875</v>
+        <v>32.167734346602984</v>
       </c>
       <c r="H22" s="2">
-        <v>7.0304788649913821</v>
+        <v>44.137686825270706</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -6599,22 +6616,22 @@
         <v>2</v>
       </c>
       <c r="C23" s="2">
-        <v>3475980</v>
+        <v>218755.41</v>
       </c>
       <c r="D23" s="2">
-        <v>33.340033619067277</v>
+        <v>44.536640205828284</v>
       </c>
       <c r="E23" s="2">
-        <v>12.130059341268209</v>
+        <v>38.034582295793612</v>
       </c>
       <c r="F23" s="2">
-        <v>159467479</v>
+        <v>13335353.310000001</v>
       </c>
       <c r="G23" s="2">
-        <v>6.4520274068071037</v>
+        <v>14.396585886905022</v>
       </c>
       <c r="H23" s="2">
-        <v>4.2571650906074785</v>
+        <v>42.0185789621857</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -6626,22 +6643,22 @@
         <v>3</v>
       </c>
       <c r="C24" s="2">
-        <v>11020048</v>
+        <v>582156.63</v>
       </c>
       <c r="D24" s="2">
-        <v>22.698349870259872</v>
+        <v>30.978809708102251</v>
       </c>
       <c r="E24" s="2">
-        <v>9.1381636822512764</v>
+        <v>35.904101434994978</v>
       </c>
       <c r="F24" s="2">
-        <v>383216515</v>
+        <v>23561140.93</v>
       </c>
       <c r="G24" s="2">
-        <v>4.3743371463214498</v>
+        <v>12.05470350920843</v>
       </c>
       <c r="H24" s="2">
-        <v>1.1327155365247801</v>
+        <v>39.592948218836639</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -6653,22 +6670,22 @@
         <v>4</v>
       </c>
       <c r="C25" s="2">
-        <v>2645230</v>
+        <v>166979.62</v>
       </c>
       <c r="D25" s="2">
-        <v>41.756035763358199</v>
+        <v>50.929804917043555</v>
       </c>
       <c r="E25" s="2">
-        <v>5.8048335832514129</v>
+        <v>33.533626346128457</v>
       </c>
       <c r="F25" s="2">
-        <v>141664497</v>
+        <v>12541986.689999999</v>
       </c>
       <c r="G25" s="2">
-        <v>12.162285139559614</v>
+        <v>18.733134495103656</v>
       </c>
       <c r="H25" s="2">
-        <v>-2.2935165674637119</v>
+        <v>36.944739246639188</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -6679,22 +6696,22 @@
         <v>1</v>
       </c>
       <c r="C26" s="2">
-        <v>1912310.9432079997</v>
+        <v>123407.0170800772</v>
       </c>
       <c r="D26" s="2">
-        <v>58.58179800262544</v>
+        <v>54.797835462364745</v>
       </c>
       <c r="E26" s="2">
-        <v>2.1745748233495883</v>
+        <v>30.967696420905892</v>
       </c>
       <c r="F26" s="2">
-        <v>142177115</v>
+        <v>11678624.99</v>
       </c>
       <c r="G26" s="2">
-        <v>20.760604587519893</v>
+        <v>25.42091904291275</v>
       </c>
       <c r="H26" s="2">
-        <v>-5.9701519780588734</v>
+        <v>34.140685294065477</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -6706,22 +6723,22 @@
         <v>2</v>
       </c>
       <c r="C27" s="2">
-        <v>2656632.5068739997</v>
+        <v>200301.74878996433</v>
       </c>
       <c r="D27" s="2">
-        <v>-23.571697568052763</v>
+        <v>-8.4357507821341109</v>
       </c>
       <c r="E27" s="2">
-        <v>-1.685637317010658</v>
+        <v>28.261723662645952</v>
       </c>
       <c r="F27" s="2">
-        <v>147146989</v>
+        <v>13858416.689999999</v>
       </c>
       <c r="G27" s="2">
-        <v>-7.7260204257696969</v>
+        <v>3.9223811161250621</v>
       </c>
       <c r="H27" s="2">
-        <v>-9.8367765758946906</v>
+        <v>31.236137356617945</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -6733,31 +6750,50 @@
         <v>3</v>
       </c>
       <c r="C28" s="2">
-        <v>1688375</v>
+        <v>497636.00198727683</v>
       </c>
       <c r="D28" s="2">
-        <v>-84.679059474151103</v>
+        <v>-14.518537393059184</v>
       </c>
       <c r="E28" s="2">
-        <v>-5.6735730428987399</v>
+        <v>25.486013911568222</v>
       </c>
       <c r="F28" s="2">
-        <v>60413605</v>
+        <v>24544442.809999999</v>
       </c>
       <c r="G28" s="2">
-        <v>-84.235124887558669</v>
+        <v>4.1734051968085106</v>
       </c>
       <c r="H28" s="2">
-        <v>-13.816269518751662</v>
+        <v>28.280996575892051</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="4"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="A29" s="1">
+        <f>A28</f>
+        <v>2024</v>
+      </c>
+      <c r="B29" s="2">
+        <v>4</v>
+      </c>
+      <c r="C29" s="2">
+        <v>145106.322522976</v>
+      </c>
+      <c r="D29" s="2">
+        <v>-13.09938151555501</v>
+      </c>
+      <c r="E29" s="2">
+        <v>22.68793708636429</v>
+      </c>
+      <c r="F29" s="2">
+        <v>12151631.66</v>
+      </c>
+      <c r="G29" s="2">
+        <v>-3.1123859373191509</v>
+      </c>
+      <c r="H29" s="2">
+        <v>25.308092995832936</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="str">
@@ -7458,29 +7494,29 @@
     <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="64.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="64.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>86</v>
       </c>
     </row>
@@ -8470,8 +8506,8 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:H53"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -8482,29 +8518,29 @@
     <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="54" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>92</v>
       </c>
     </row>
@@ -8535,6 +8571,9 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2018</v>
+      </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
@@ -8558,6 +8597,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2018</v>
+      </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
@@ -8581,6 +8623,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2018</v>
+      </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
@@ -8630,6 +8675,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2019</v>
+      </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
@@ -8653,6 +8701,9 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2019</v>
+      </c>
       <c r="B8" s="1">
         <v>3</v>
       </c>
@@ -8676,6 +8727,9 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2019</v>
+      </c>
       <c r="B9" s="1">
         <v>4</v>
       </c>
@@ -8725,6 +8779,9 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>2020</v>
+      </c>
       <c r="B11" s="1">
         <v>2</v>
       </c>
@@ -8748,6 +8805,9 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>2020</v>
+      </c>
       <c r="B12" s="1">
         <v>3</v>
       </c>
@@ -8771,6 +8831,9 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>2020</v>
+      </c>
       <c r="B13" s="1">
         <v>4</v>
       </c>
@@ -8820,6 +8883,9 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>2021</v>
+      </c>
       <c r="B15" s="1">
         <v>2</v>
       </c>
@@ -8843,6 +8909,9 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>2021</v>
+      </c>
       <c r="B16" s="1">
         <v>3</v>
       </c>
@@ -8866,6 +8935,9 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>2021</v>
+      </c>
       <c r="B17" s="1">
         <v>4</v>
       </c>
@@ -8915,6 +8987,9 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>2022</v>
+      </c>
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -8938,6 +9013,9 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>2022</v>
+      </c>
       <c r="B20" s="1">
         <v>3</v>
       </c>
@@ -8961,6 +9039,9 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>2022</v>
+      </c>
       <c r="B21" s="1">
         <v>4</v>
       </c>
@@ -9010,6 +9091,9 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>2023</v>
+      </c>
       <c r="B23" s="1">
         <v>2</v>
       </c>
@@ -9033,6 +9117,9 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>2023</v>
+      </c>
       <c r="B24" s="1">
         <v>3</v>
       </c>
@@ -9056,6 +9143,9 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>2023</v>
+      </c>
       <c r="B25" s="1">
         <v>4</v>
       </c>
@@ -9105,6 +9195,9 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>2024</v>
+      </c>
       <c r="B27" s="1">
         <v>2</v>
       </c>
@@ -9128,6 +9221,9 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>2024</v>
+      </c>
       <c r="B28" s="1">
         <v>3</v>
       </c>
@@ -9151,6 +9247,9 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>2024</v>
+      </c>
       <c r="B29" s="1">
         <v>4</v>
       </c>
@@ -9185,7 +9284,7 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H54" sqref="A30:H54"/>
     </sheetView>
   </sheetViews>
@@ -9197,29 +9296,29 @@
     <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>98</v>
       </c>
     </row>
@@ -10220,29 +10319,29 @@
     <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="64.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="64.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -11675,29 +11774,29 @@
     <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="75.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="75.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -12193,10 +12292,10 @@
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="5"/>
+      <c r="C29" s="4"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="5"/>
+      <c r="F29" s="4"/>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -12898,29 +12997,29 @@
     <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="54" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -13923,29 +14022,29 @@
     <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="54" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -14947,29 +15046,29 @@
     <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -15971,29 +16070,29 @@
     <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="64.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="64.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>44</v>
       </c>
     </row>
@@ -16994,29 +17093,29 @@
     <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="54" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>50</v>
       </c>
     </row>
@@ -18449,29 +18548,29 @@
     <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="54" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización 17/06/2025 2  #62333
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_trimestral.xlsx
+++ b/etl/data/input/Datos_carga_trimestral.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\economia\1. Publicaciones\Panel indicadores economicos\envio_informatica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sp-fs-200.ad2.cantabria.es\G2R00001\datos\publicaciones\Panel indicadores socioeconomicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" tabRatio="820" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" tabRatio="820" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="PIB" sheetId="33" r:id="rId1"/>
@@ -1600,7 +1600,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:H33"/>
+      <selection activeCell="H33" sqref="A31:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -2413,89 +2413,35 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <f t="shared" ref="A31:A54" si="1">IF(C31="","",A30)</f>
-        <v>2025</v>
-      </c>
-      <c r="B31" s="2">
-        <v>2</v>
-      </c>
-      <c r="C31" s="2">
-        <v>0</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0</v>
-      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <f t="shared" si="1"/>
-        <v>2025</v>
-      </c>
-      <c r="B32" s="2">
-        <v>3</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0</v>
-      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <f t="shared" si="1"/>
-        <v>2025</v>
-      </c>
-      <c r="B33" s="2">
-        <v>4</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0</v>
-      </c>
-      <c r="E33" s="2">
-        <v>0</v>
-      </c>
-      <c r="F33" s="2">
-        <v>0</v>
-      </c>
-      <c r="G33" s="2">
-        <v>0</v>
-      </c>
-      <c r="H33" s="2">
-        <v>0</v>
-      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A31:A54" si="1">IF(C34="","",A33)</f>
         <v/>
       </c>
       <c r="B34" s="1" t="s">
@@ -3072,8 +3018,8 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:H33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H33" sqref="A31:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -3891,89 +3837,32 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <f t="shared" ref="A31:A54" si="1">IF(C31="","",A30)</f>
-        <v>2025</v>
-      </c>
-      <c r="B31" s="1">
-        <v>2</v>
-      </c>
-      <c r="C31" s="4">
-        <v>0</v>
-      </c>
-      <c r="D31" s="4">
-        <v>0</v>
-      </c>
-      <c r="E31" s="4">
-        <v>0</v>
-      </c>
-      <c r="F31" s="4">
-        <v>0</v>
-      </c>
-      <c r="G31" s="4">
-        <v>0</v>
-      </c>
-      <c r="H31" s="4">
-        <v>0</v>
-      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <f t="shared" si="1"/>
-        <v>2025</v>
-      </c>
-      <c r="B32" s="1">
-        <v>3</v>
-      </c>
-      <c r="C32" s="4">
-        <v>0</v>
-      </c>
-      <c r="D32" s="4">
-        <v>0</v>
-      </c>
-      <c r="E32" s="4">
-        <v>0</v>
-      </c>
-      <c r="F32" s="4">
-        <v>0</v>
-      </c>
-      <c r="G32" s="4">
-        <v>0</v>
-      </c>
-      <c r="H32" s="4">
-        <v>0</v>
-      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <f t="shared" si="1"/>
-        <v>2025</v>
-      </c>
-      <c r="B33" s="1">
-        <v>4</v>
-      </c>
-      <c r="C33" s="4">
-        <v>0</v>
-      </c>
-      <c r="D33" s="4">
-        <v>0</v>
-      </c>
-      <c r="E33" s="4">
-        <v>0</v>
-      </c>
-      <c r="F33" s="4">
-        <v>0</v>
-      </c>
-      <c r="G33" s="4">
-        <v>0</v>
-      </c>
-      <c r="H33" s="4">
-        <v>0</v>
-      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A31:A54" si="1">IF(C34="","",A33)</f>
         <v/>
       </c>
       <c r="B34" s="1" t="s">
@@ -5365,7 +5254,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="str">
-        <f t="shared" ref="A31:A54" si="1">IF(C33="","",A32)</f>
+        <f t="shared" ref="A33:A54" si="1">IF(C33="","",A32)</f>
         <v/>
       </c>
       <c r="B33" s="1" t="s">
@@ -9291,7 +9180,7 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -13024,7 +12913,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:A33"/>
+      <selection activeCell="H33" sqref="A31:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -13837,87 +13726,33 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <f>A30</f>
-        <v>2025</v>
-      </c>
-      <c r="B31" s="2">
-        <v>2</v>
-      </c>
-      <c r="C31" s="2">
-        <v>0</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0</v>
-      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <f t="shared" ref="A32:A33" si="1">A31</f>
-        <v>2025</v>
-      </c>
-      <c r="B32" s="2">
-        <v>3</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <f t="shared" si="1"/>
-        <v>2025</v>
-      </c>
-      <c r="B33" s="2">
-        <v>4</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0</v>
-      </c>
-      <c r="E33" s="2">
-        <v>0</v>
-      </c>
-      <c r="F33" s="2">
-        <v>0</v>
-      </c>
-      <c r="G33" s="2">
-        <v>0</v>
-      </c>
-      <c r="H33" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -13926,7 +13761,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -13935,7 +13770,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -13944,7 +13779,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -13953,7 +13788,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -13962,7 +13797,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -13971,7 +13806,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -13980,7 +13815,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -13989,7 +13824,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -13998,7 +13833,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -14007,7 +13842,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -14016,7 +13851,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -14025,7 +13860,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -14034,7 +13869,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -14043,7 +13878,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -14120,7 +13955,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="I40" sqref="I40:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -14933,87 +14768,33 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <f>A30</f>
-        <v>2025</v>
-      </c>
-      <c r="B31" s="2">
-        <v>2</v>
-      </c>
-      <c r="C31" s="2">
-        <v>0</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0</v>
-      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <f t="shared" ref="A32:A33" si="1">A31</f>
-        <v>2025</v>
-      </c>
-      <c r="B32" s="2">
-        <v>3</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <f t="shared" si="1"/>
-        <v>2025</v>
-      </c>
-      <c r="B33" s="2">
-        <v>4</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0</v>
-      </c>
-      <c r="E33" s="2">
-        <v>0</v>
-      </c>
-      <c r="F33" s="2">
-        <v>0</v>
-      </c>
-      <c r="G33" s="2">
-        <v>0</v>
-      </c>
-      <c r="H33" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -15022,7 +14803,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -15031,7 +14812,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -15040,7 +14821,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -15049,7 +14830,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -15058,7 +14839,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -15067,7 +14848,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -15076,7 +14857,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -15085,7 +14866,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -15094,7 +14875,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -15103,7 +14884,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -15112,7 +14893,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -15121,7 +14902,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -15130,7 +14911,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -15139,7 +14920,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -15215,7 +14996,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:A33"/>
+      <selection activeCell="I40" sqref="I40:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -16028,87 +15809,33 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <f>A30</f>
-        <v>2025</v>
-      </c>
-      <c r="B31" s="2">
-        <v>2</v>
-      </c>
-      <c r="C31" s="2">
-        <v>0</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0</v>
-      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <f>A31</f>
-        <v>2025</v>
-      </c>
-      <c r="B32" s="2">
-        <v>3</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <f>A32</f>
-        <v>2025</v>
-      </c>
-      <c r="B33" s="2">
-        <v>4</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0</v>
-      </c>
-      <c r="E33" s="2">
-        <v>0</v>
-      </c>
-      <c r="F33" s="2">
-        <v>0</v>
-      </c>
-      <c r="G33" s="2">
-        <v>0</v>
-      </c>
-      <c r="H33" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -16117,7 +15844,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -16126,7 +15853,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -16135,7 +15862,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -16144,7 +15871,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -16153,7 +15880,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -16162,7 +15889,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -16171,7 +15898,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -16180,7 +15907,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -16189,7 +15916,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -16198,7 +15925,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -16207,7 +15934,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -16216,7 +15943,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -16225,7 +15952,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -16234,7 +15961,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -16310,7 +16037,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="I40" sqref="I40:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -17123,87 +16850,33 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <f>A30</f>
-        <v>2025</v>
-      </c>
-      <c r="B31" s="2">
-        <v>2</v>
-      </c>
-      <c r="C31" s="2">
-        <v>0</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0</v>
-      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <f t="shared" ref="A32:A33" si="1">A31</f>
-        <v>2025</v>
-      </c>
-      <c r="B32" s="2">
-        <v>3</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <f t="shared" si="1"/>
-        <v>2025</v>
-      </c>
-      <c r="B33" s="2">
-        <v>4</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0</v>
-      </c>
-      <c r="E33" s="2">
-        <v>0</v>
-      </c>
-      <c r="F33" s="2">
-        <v>0</v>
-      </c>
-      <c r="G33" s="2">
-        <v>0</v>
-      </c>
-      <c r="H33" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -17212,7 +16885,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -17221,7 +16894,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -17230,7 +16903,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -17239,7 +16912,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -17248,7 +16921,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -17257,7 +16930,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -17266,7 +16939,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -17275,7 +16948,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -17284,7 +16957,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -17293,7 +16966,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -17302,7 +16975,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -17311,7 +16984,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -17320,7 +16993,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -17329,7 +17002,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -17405,7 +17078,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:H33"/>
+      <selection activeCell="I40" sqref="I40:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -18217,89 +17890,35 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <f>A30</f>
-        <v>2025</v>
-      </c>
-      <c r="B31" s="2">
-        <v>2</v>
-      </c>
-      <c r="C31" s="2">
-        <v>0</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0</v>
-      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <f t="shared" ref="A32:A33" si="1">A31</f>
-        <v>2025</v>
-      </c>
-      <c r="B32" s="2">
-        <v>3</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0</v>
-      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <f t="shared" si="1"/>
-        <v>2025</v>
-      </c>
-      <c r="B33" s="2">
-        <v>4</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0</v>
-      </c>
-      <c r="E33" s="2">
-        <v>0</v>
-      </c>
-      <c r="F33" s="2">
-        <v>0</v>
-      </c>
-      <c r="G33" s="2">
-        <v>0</v>
-      </c>
-      <c r="H33" s="2">
-        <v>0</v>
-      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="str">
-        <f t="shared" ref="A34:A54" si="2">IF(C34="","",A33)</f>
+        <f t="shared" ref="A34:A54" si="1">IF(C34="","",A33)</f>
         <v/>
       </c>
       <c r="B34" s="1" t="s">
@@ -18326,7 +17945,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B35" s="1" t="s">
@@ -18353,7 +17972,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B36" s="1" t="s">
@@ -18380,7 +17999,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B37" s="1" t="s">
@@ -18407,7 +18026,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B38" s="1" t="s">
@@ -18434,7 +18053,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B39" s="1" t="s">
@@ -18461,7 +18080,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B40" s="1" t="s">
@@ -18488,7 +18107,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B41" s="1" t="s">
@@ -18515,7 +18134,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B42" s="1" t="s">
@@ -18542,7 +18161,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B43" s="1" t="s">
@@ -18569,7 +18188,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B44" s="1" t="s">
@@ -18596,7 +18215,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B45" s="1" t="s">
@@ -18623,7 +18242,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B46" s="1" t="s">
@@ -18650,7 +18269,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B47" s="1" t="s">
@@ -18677,7 +18296,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B48" s="1" t="s">
@@ -18704,7 +18323,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B49" s="1" t="s">
@@ -18731,7 +18350,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B50" s="1" t="s">
@@ -18758,7 +18377,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B51" s="1" t="s">
@@ -18785,7 +18404,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B52" s="1" t="s">
@@ -18812,7 +18431,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B53" s="1" t="s">
@@ -18839,7 +18458,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B54" s="1" t="s">

</xml_diff>

<commit_message>
Actualización 17/06/2025 3  #62333
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_trimestral.xlsx
+++ b/etl/data/input/Datos_carga_trimestral.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" tabRatio="820" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" tabRatio="820" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="PIB" sheetId="33" r:id="rId1"/>
@@ -2441,7 +2441,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="str">
-        <f t="shared" ref="A31:A54" si="1">IF(C34="","",A33)</f>
+        <f t="shared" ref="A34:A54" si="1">IF(C34="","",A33)</f>
         <v/>
       </c>
       <c r="B34" s="1" t="s">
@@ -3018,7 +3018,7 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H33" sqref="A31:H33"/>
     </sheetView>
   </sheetViews>
@@ -3862,7 +3862,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="str">
-        <f t="shared" ref="A31:A54" si="1">IF(C34="","",A33)</f>
+        <f t="shared" ref="A34:A54" si="1">IF(C34="","",A33)</f>
         <v/>
       </c>
       <c r="B34" s="1" t="s">
@@ -5859,7 +5859,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="H32" sqref="A30:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -6646,88 +6646,35 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>2025</v>
-      </c>
-      <c r="B30" s="2">
-        <v>1</v>
-      </c>
-      <c r="C30" s="2">
-        <v>0</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0</v>
-      </c>
-      <c r="F30" s="2">
-        <v>0</v>
-      </c>
-      <c r="G30" s="2">
-        <v>0</v>
-      </c>
-      <c r="H30" s="2">
-        <v>0</v>
-      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <f t="shared" ref="A31:A54" si="1">IF(C31="","",A30)</f>
-        <v>2025</v>
-      </c>
-      <c r="B31" s="2">
-        <v>2</v>
-      </c>
-      <c r="C31" s="2">
-        <v>0</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0</v>
-      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <f t="shared" si="1"/>
-        <v>2025</v>
-      </c>
-      <c r="B32" s="2">
-        <v>3</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0</v>
-      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A33:A54" si="1">IF(C33="","",A32)</f>
         <v/>
       </c>
       <c r="B33" s="1" t="s">
@@ -16036,7 +15983,7 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I40" sqref="I40:I41"/>
     </sheetView>
   </sheetViews>
@@ -18496,7 +18443,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:A33"/>
+      <selection activeCell="A33" sqref="A33:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -19362,34 +19309,15 @@
         <v>4.0473868530415569</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <f t="shared" si="2"/>
-        <v>2025</v>
-      </c>
-      <c r="B33" s="1">
-        <v>4</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0</v>
-      </c>
-      <c r="E33" s="2">
-        <v>0</v>
-      </c>
-      <c r="F33" s="2">
-        <v>0</v>
-      </c>
-      <c r="G33" s="2">
-        <v>0</v>
-      </c>
-      <c r="H33" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -19397,7 +19325,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -19405,7 +19333,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -19413,7 +19341,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -19421,7 +19349,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -19429,7 +19357,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -19437,7 +19365,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -19445,7 +19373,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -19453,7 +19381,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -19461,7 +19389,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -19469,7 +19397,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -19477,7 +19405,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -19485,7 +19413,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -19493,7 +19421,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -19501,7 +19429,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>

</xml_diff>

<commit_message>
Actualiza datos según tarea redmine #67339
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_trimestral.xlsx
+++ b/etl/data/input/Datos_carga_trimestral.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\economia\1. Publicaciones\Panel indicadores economicos\envio_informatica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\economia\1. Publicaciones\Panel indicadores economicos\0. Viejo\envio_informatica\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" tabRatio="820" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" tabRatio="820" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="PIB" sheetId="33" r:id="rId1"/>
@@ -29,9 +29,6 @@
     <sheet name="IPV" sheetId="24" r:id="rId15"/>
     <sheet name="TI" sheetId="25" r:id="rId16"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId17"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -410,135 +407,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="PIB"/>
-      <sheetName val="DEUDA"/>
-      <sheetName val="DEUDA_PIB"/>
-      <sheetName val="PCN"/>
-      <sheetName val="PCN_PIB"/>
-      <sheetName val="Afi"/>
-      <sheetName val="Afi_asa"/>
-      <sheetName val="Afi_noasa"/>
-      <sheetName val="Paro"/>
-      <sheetName val="Contra"/>
-      <sheetName val="EPA"/>
-      <sheetName val="EPA_2"/>
-      <sheetName val="EPA_3"/>
-      <sheetName val="EPA_4"/>
-      <sheetName val="EPA_5"/>
-      <sheetName val="Emp"/>
-      <sheetName val="Emp_fi"/>
-      <sheetName val="Emp_ju"/>
-      <sheetName val="ICE"/>
-      <sheetName val="SM_C"/>
-      <sheetName val="SM_D"/>
-      <sheetName val="IPI"/>
-      <sheetName val="ICN"/>
-      <sheetName val="ECI"/>
-      <sheetName val="Matr"/>
-      <sheetName val="CP"/>
-      <sheetName val="CGN"/>
-      <sheetName val="ENERGÍA"/>
-      <sheetName val="IPV"/>
-      <sheetName val="TI"/>
-      <sheetName val="CEMENTO"/>
-      <sheetName val="LOC"/>
-      <sheetName val="IASS"/>
-      <sheetName val="IASS_2"/>
-      <sheetName val="ICM"/>
-      <sheetName val="ICM_2"/>
-      <sheetName val="Taereo"/>
-      <sheetName val="TPS_P"/>
-      <sheetName val="TPS_M"/>
-      <sheetName val="TMC"/>
-      <sheetName val="CTH"/>
-      <sheetName val="EOAT"/>
-      <sheetName val="ETR_5"/>
-      <sheetName val="ETR_6"/>
-      <sheetName val="EGATUR"/>
-      <sheetName val="FRONTUR"/>
-      <sheetName val="Ipc"/>
-      <sheetName val="PRD_G"/>
-      <sheetName val="PRD_B"/>
-      <sheetName val="P_CONTR"/>
-      <sheetName val="P_NO_CONTR"/>
-      <sheetName val="GS"/>
-      <sheetName val="X"/>
-      <sheetName val="M"/>
-      <sheetName val="SALDO"/>
-      <sheetName val="TCOBER"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18">
-        <row r="2">
-          <cell r="B2">
-            <v>1</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -3176,7 +3044,7 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
@@ -18529,8 +18397,8 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -18572,7 +18440,6 @@
         <v>2018</v>
       </c>
       <c r="B2" s="1">
-        <f>[1]ICE!B2</f>
         <v>1</v>
       </c>
       <c r="C2" s="2">
@@ -18582,7 +18449,7 @@
         <v>6.0966542750929387</v>
       </c>
       <c r="E2" s="2">
-        <v>0.99514182287635289</v>
+        <v>0.99950034426208856</v>
       </c>
       <c r="F2" s="2">
         <v>134.9</v>
@@ -18591,12 +18458,11 @@
         <v>2.3520485584218376</v>
       </c>
       <c r="H2" s="2">
-        <v>-7.0463435267163171E-2</v>
+        <v>-5.2571570733197487E-2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <f>A2</f>
         <v>2018</v>
       </c>
       <c r="B3" s="1">
@@ -18609,7 +18475,7 @@
         <v>0.6382978723404209</v>
       </c>
       <c r="E3" s="2">
-        <v>0.531969600164516</v>
+        <v>0.53697451168734389</v>
       </c>
       <c r="F3" s="2">
         <v>135.5</v>
@@ -18618,12 +18484,11 @@
         <v>0.96870342771981921</v>
       </c>
       <c r="H3" s="2">
-        <v>-0.49328927849431636</v>
+        <v>-0.47274396253831674</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <f>A3</f>
         <v>2018</v>
       </c>
       <c r="B4" s="1">
@@ -18636,7 +18501,7 @@
         <v>-2.3411371237458178</v>
       </c>
       <c r="E4" s="2">
-        <v>0.12031001222628278</v>
+        <v>0.12598270154100913</v>
       </c>
       <c r="F4" s="2">
         <v>136.19999999999999</v>
@@ -18645,12 +18510,11 @@
         <v>-0.51132213294377005</v>
       </c>
       <c r="H4" s="2">
-        <v>-0.8578801928127644</v>
+        <v>-0.83459362845299645</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <f>A4</f>
         <v>2018</v>
       </c>
       <c r="B5" s="1">
@@ -18663,7 +18527,7 @@
         <v>0.76655052264809065</v>
       </c>
       <c r="E5" s="2">
-        <v>-0.23120438571353158</v>
+        <v>-0.22485389237343417</v>
       </c>
       <c r="F5" s="2">
         <v>133.9</v>
@@ -18672,7 +18536,7 @@
         <v>-1.107828655834564</v>
       </c>
       <c r="H5" s="2">
-        <v>-1.157312000420984</v>
+        <v>-1.1312430296602274</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -18689,7 +18553,7 @@
         <v>-2.3125437981779795</v>
       </c>
       <c r="E6" s="2">
-        <v>-0.51547944289009451</v>
+        <v>-0.50845602614330865</v>
       </c>
       <c r="F6" s="2">
         <v>132.5</v>
@@ -18698,12 +18562,11 @@
         <v>-1.779095626389926</v>
       </c>
       <c r="H6" s="2">
-        <v>-1.3844439247300337</v>
+        <v>-1.355612582658307</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <f>A6</f>
         <v>2019</v>
       </c>
       <c r="B7" s="1">
@@ -18716,7 +18579,7 @@
         <v>-1.6913319238900715</v>
       </c>
       <c r="E7" s="2">
-        <v>-0.72479741172084744</v>
+        <v>-0.71712482809654854</v>
       </c>
       <c r="F7" s="2">
         <v>132.9</v>
@@ -18725,12 +18588,11 @@
         <v>-1.9188191881918781</v>
       </c>
       <c r="H7" s="2">
-        <v>-1.5321042620606058</v>
+        <v>-1.5006080699618916</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <f>A7</f>
         <v>2019</v>
       </c>
       <c r="B8" s="1">
@@ -18743,7 +18605,7 @@
         <v>-0.54794520547946091</v>
       </c>
       <c r="E8" s="2">
-        <v>-0.85256370984528673</v>
+        <v>-0.84428898141860975</v>
       </c>
       <c r="F8" s="2">
         <v>135</v>
@@ -18752,12 +18614,11 @@
         <v>-0.88105726872246271</v>
       </c>
       <c r="H8" s="2">
-        <v>-1.5933679660469295</v>
+        <v>-1.5593999509879699</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <f>A8</f>
         <v>2019</v>
       </c>
       <c r="B9" s="1">
@@ -18770,7 +18631,7 @@
         <v>-1.1756569847856113</v>
       </c>
       <c r="E9" s="2">
-        <v>-0.89278783897301439</v>
+        <v>-0.88398604872981912</v>
       </c>
       <c r="F9" s="2">
         <v>131.1</v>
@@ -18779,7 +18640,7 @@
         <v>-2.0911127707244348</v>
       </c>
       <c r="H9" s="2">
-        <v>-1.5615516871520665</v>
+        <v>-1.5254200671024245</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -18796,7 +18657,7 @@
         <v>-3.0846484935437624</v>
       </c>
       <c r="E10" s="2">
-        <v>-0.83928891424840391</v>
+        <v>-0.83006837779054143</v>
       </c>
       <c r="F10" s="2">
         <v>130.6</v>
@@ -18805,12 +18666,11 @@
         <v>-1.4339622641509453</v>
       </c>
       <c r="H10" s="2">
-        <v>-1.4295268816532505</v>
+        <v>-1.3916762954947217</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <f>A10</f>
         <v>2020</v>
       </c>
       <c r="B11" s="1">
@@ -18823,7 +18683,7 @@
         <v>-27.670250896057347</v>
       </c>
       <c r="E11" s="2">
-        <v>-0.68606284403196183</v>
+        <v>-0.67657061069617663</v>
       </c>
       <c r="F11" s="2">
         <v>95.5</v>
@@ -18832,12 +18692,11 @@
         <v>-28.14145974416855</v>
       </c>
       <c r="H11" s="2">
-        <v>-1.1904959815049485</v>
+        <v>-1.1515300712940921</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <f>A11</f>
         <v>2020</v>
       </c>
       <c r="B12" s="1">
@@ -18850,7 +18709,7 @@
         <v>-27.96143250688705</v>
       </c>
       <c r="E12" s="2">
-        <v>-0.42850888642125423</v>
+        <v>-0.41893650211447042</v>
       </c>
       <c r="F12" s="2">
         <v>95.5</v>
@@ -18859,12 +18718,11 @@
         <v>-29.259259259259263</v>
       </c>
       <c r="H12" s="2">
-        <v>-0.83766419077568843</v>
+        <v>-0.79836925836017647</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <f>A12</f>
         <v>2020</v>
       </c>
       <c r="B13" s="1">
@@ -18877,7 +18735,7 @@
         <v>-14.97550734779567</v>
       </c>
       <c r="E13" s="2">
-        <v>-7.8891417046363141E-2</v>
+        <v>-6.9480856891519296E-2</v>
       </c>
       <c r="F13" s="2">
         <v>105.5</v>
@@ -18886,7 +18744,7 @@
         <v>-19.527078565980162</v>
       </c>
       <c r="H13" s="2">
-        <v>-0.3810810658856631</v>
+        <v>-0.34245042659816205</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -18903,7 +18761,7 @@
         <v>-10.65877128053293</v>
       </c>
       <c r="E14" s="2">
-        <v>0.33331711119983826</v>
+        <v>0.34226746012359738</v>
       </c>
       <c r="F14" s="2">
         <v>109.3</v>
@@ -18912,12 +18770,11 @@
         <v>-16.309341500765694</v>
       </c>
       <c r="H14" s="2">
-        <v>0.15144033982713256</v>
+        <v>0.18818179783620168</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <f t="shared" ref="A15:A25" si="0">A14</f>
         <v>2021</v>
       </c>
       <c r="B15" s="1">
@@ -18930,7 +18787,7 @@
         <v>28.047571853320097</v>
       </c>
       <c r="E15" s="2">
-        <v>0.76933386046775842</v>
+        <v>0.7774633175249851</v>
       </c>
       <c r="F15" s="2">
         <v>114.8</v>
@@ -18939,12 +18796,11 @@
         <v>20.209424083769623</v>
       </c>
       <c r="H15" s="2">
-        <v>0.72012072458714438</v>
+        <v>0.7534923962000516</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <f t="shared" si="0"/>
         <v>2021</v>
       </c>
       <c r="B16" s="1">
@@ -18957,7 +18813,7 @@
         <v>33.365200764818368</v>
       </c>
       <c r="E16" s="2">
-        <v>1.1835059376629729</v>
+        <v>1.190385934693839</v>
       </c>
       <c r="F16" s="2">
         <v>128.9</v>
@@ -18966,12 +18822,11 @@
         <v>34.973821989528808</v>
       </c>
       <c r="H16" s="2">
-        <v>1.2748927979684477</v>
+        <v>1.3031353976888984</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <f t="shared" si="0"/>
         <v>2021</v>
       </c>
       <c r="B17" s="1">
@@ -18984,7 +18839,7 @@
         <v>15.7201646090535</v>
       </c>
       <c r="E17" s="2">
-        <v>1.54722934843659</v>
+        <v>1.5523583488462265</v>
       </c>
       <c r="F17" s="2">
         <v>130.30000000000001</v>
@@ -18993,7 +18848,7 @@
         <v>23.507109004739355</v>
       </c>
       <c r="H17" s="2">
-        <v>1.7778700841446071</v>
+        <v>1.798924788802984</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -19010,7 +18865,7 @@
         <v>12.013256006627993</v>
       </c>
       <c r="E18" s="2">
-        <v>1.8520136577066901</v>
+        <v>1.8548128564670423</v>
       </c>
       <c r="F18" s="2">
         <v>127</v>
@@ -19019,12 +18874,11 @@
         <v>16.193961573650519</v>
       </c>
       <c r="H18" s="2">
-        <v>2.2122279380339123</v>
+        <v>2.2237187351624499</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <f>A18</f>
         <v>2022</v>
       </c>
       <c r="B19" s="1">
@@ -19037,7 +18891,7 @@
         <v>1.702786377708998</v>
       </c>
       <c r="E19" s="2">
-        <v>2.0982265149292392</v>
+        <v>2.0980366329538112</v>
       </c>
       <c r="F19" s="2">
         <v>121.9</v>
@@ -19046,12 +18900,11 @@
         <v>6.1846689895470375</v>
       </c>
       <c r="H19" s="2">
-        <v>2.5747224888800244</v>
+        <v>2.5739430175223981</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <f t="shared" si="0"/>
         <v>2022</v>
       </c>
       <c r="B20" s="1">
@@ -19064,7 +18917,7 @@
         <v>-1.5053763440860179</v>
       </c>
       <c r="E20" s="2">
-        <v>2.2925863460282789</v>
+        <v>2.2886658806729083</v>
       </c>
       <c r="F20" s="2">
         <v>131</v>
@@ -19073,12 +18926,11 @@
         <v>1.6291698991466319</v>
       </c>
       <c r="H20" s="2">
-        <v>2.8708484494488653</v>
+        <v>2.8547548184119855</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <f t="shared" si="0"/>
         <v>2022</v>
       </c>
       <c r="B21" s="1">
@@ -19091,7 +18943,7 @@
         <v>-0.64011379800853474</v>
       </c>
       <c r="E21" s="2">
-        <v>2.4415644268420884</v>
+        <v>2.4330897705811805</v>
       </c>
       <c r="F21" s="2">
         <v>127.2</v>
@@ -19100,7 +18952,7 @@
         <v>-2.3791250959324661</v>
       </c>
       <c r="H21" s="2">
-        <v>3.1083567490692734</v>
+        <v>3.073568024092884</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -19117,7 +18969,7 @@
         <v>2.4408284023668791</v>
       </c>
       <c r="E22" s="2">
-        <v>2.5492583065276251</v>
+        <v>2.5353261972450003</v>
       </c>
       <c r="F22" s="2">
         <v>129</v>
@@ -19126,12 +18978,11 @@
         <v>1.5748031496062964</v>
       </c>
       <c r="H22" s="2">
-        <v>3.2942222679761479</v>
+        <v>3.2370305302522246</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <f>A22</f>
         <v>2023</v>
       </c>
       <c r="B23" s="1">
@@ -19144,7 +18995,7 @@
         <v>6.7732115677321181</v>
       </c>
       <c r="E23" s="2">
-        <v>2.6178394853513143</v>
+        <v>2.5974723030003712</v>
       </c>
       <c r="F23" s="2">
         <v>132.5</v>
@@ -19153,12 +19004,11 @@
         <v>8.6956521739130377</v>
       </c>
       <c r="H23" s="2">
-        <v>3.4319902102512616</v>
+        <v>3.3483822993771222</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <f t="shared" si="0"/>
         <v>2023</v>
       </c>
       <c r="B24" s="1">
@@ -19171,7 +19021,7 @@
         <v>7.1324599708879166</v>
       </c>
       <c r="E24" s="2">
-        <v>2.6494116948894808</v>
+        <v>2.6215661690614982</v>
       </c>
       <c r="F24" s="2">
         <v>135.9</v>
@@ -19180,12 +19030,11 @@
         <v>3.7404580152671896</v>
       </c>
       <c r="H24" s="2">
-        <v>3.524131143027406</v>
+        <v>3.4098244018417878</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <f t="shared" si="0"/>
         <v>2023</v>
       </c>
       <c r="B25" s="1">
@@ -19198,7 +19047,7 @@
         <v>2.5053686471009362</v>
       </c>
       <c r="E25" s="2">
-        <v>2.6486757742699378</v>
+        <v>2.6122557136830435</v>
       </c>
       <c r="F25" s="2">
         <v>133.19999999999999</v>
@@ -19207,7 +19056,7 @@
         <v>4.7169811320754595</v>
       </c>
       <c r="H25" s="2">
-        <v>3.5764054221646622</v>
+        <v>3.4268999516920182</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -19224,7 +19073,7 @@
         <v>-0.14440433212995485</v>
       </c>
       <c r="E26" s="2">
-        <v>2.623134467792998</v>
+        <v>2.5770081637458113</v>
       </c>
       <c r="F26" s="2">
         <v>134</v>
@@ -19233,12 +19082,11 @@
         <v>3.8759689922480689</v>
       </c>
       <c r="H26" s="2">
-        <v>3.5947086078182604</v>
+        <v>3.4053587089820003</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <f>A26</f>
         <v>2024</v>
       </c>
       <c r="B27" s="1">
@@ -19251,7 +19099,7 @@
         <v>2.2095509622237941</v>
       </c>
       <c r="E27" s="2">
-        <v>2.5802009528044931</v>
+        <v>2.5232239417139919</v>
       </c>
       <c r="F27" s="2">
         <v>136</v>
@@ -19260,12 +19108,11 @@
         <v>2.6415094339622636</v>
       </c>
       <c r="H27" s="2">
-        <v>3.5856491199621261</v>
+        <v>3.3517567345036614</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <f t="shared" ref="A28:A29" si="1">A27</f>
         <v>2024</v>
       </c>
       <c r="B28" s="1">
@@ -19278,7 +19125,7 @@
         <v>-0.747282608695643</v>
       </c>
       <c r="E28" s="2">
-        <v>2.5255586949003037</v>
+        <v>2.4566025872418535</v>
       </c>
       <c r="F28" s="2">
         <v>138</v>
@@ -19287,12 +19134,11 @@
         <v>1.5452538631346435</v>
       </c>
       <c r="H28" s="2">
-        <v>3.5560111663104532</v>
+        <v>3.2729442204759707</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <f t="shared" si="1"/>
         <v>2024</v>
       </c>
       <c r="B29" s="1">
@@ -19305,7 +19151,7 @@
         <v>-1.8156424581005526</v>
       </c>
       <c r="E29" s="2">
-        <v>2.464659503432197</v>
+        <v>2.3826475943714831</v>
       </c>
       <c r="F29" s="2">
         <v>136.30000000000001</v>
@@ -19314,7 +19160,7 @@
         <v>2.3273273273273443</v>
       </c>
       <c r="H29" s="2">
-        <v>3.5119888672736863</v>
+        <v>3.1753274545550592</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -19331,7 +19177,7 @@
         <v>4.3383947939262368</v>
       </c>
       <c r="E30" s="2">
-        <v>2.400909661937193</v>
+        <v>2.3048600288975067</v>
       </c>
       <c r="F30" s="2">
         <v>137</v>
@@ -19340,12 +19186,11 @@
         <v>2.2388059701492491</v>
       </c>
       <c r="H30" s="2">
-        <v>3.458519619947785</v>
+        <v>3.0642329179237189</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <f t="shared" ref="A31:A32" si="2">IF(C31="","",A30)</f>
         <v>2025</v>
       </c>
       <c r="B31" s="1">
@@ -19358,7 +19203,7 @@
         <v>-0.48814504881451448</v>
       </c>
       <c r="E31" s="2">
-        <v>2.335040265226354</v>
+        <v>2.2241170253317555</v>
       </c>
       <c r="F31" s="2">
         <v>137.1</v>
@@ -19367,12 +19212,11 @@
         <v>0.80882352941176183</v>
       </c>
       <c r="H31" s="2">
-        <v>3.3998004079662421</v>
+        <v>2.9444570916852251</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <f t="shared" si="2"/>
         <v>2025</v>
       </c>
       <c r="B32" s="1">
@@ -19385,7 +19229,7 @@
         <v>1.9849418206707714</v>
       </c>
       <c r="E32" s="2">
-        <v>2.2689933363182355</v>
+        <v>2.1425666774142034</v>
       </c>
       <c r="F32" s="2">
         <v>138.6</v>
@@ -19394,18 +19238,36 @@
         <v>0.43478260869564966</v>
       </c>
       <c r="H32" s="2">
-        <v>3.3392658939314268</v>
-      </c>
-    </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+        <v>2.8202805651004939</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>2025</v>
+      </c>
+      <c r="B33" s="1">
+        <v>4</v>
+      </c>
+      <c r="C33" s="2">
+        <v>142.69999999999999</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1.4935988620199181</v>
+      </c>
+      <c r="E33" s="2">
+        <v>2.0606619150884833</v>
+      </c>
+      <c r="F33" s="2">
+        <v>136.80000000000001</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.3668378576669129</v>
+      </c>
+      <c r="H33" s="2">
+        <v>2.6946491564540205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -19413,7 +19275,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -19421,7 +19283,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -19429,7 +19291,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -19437,7 +19299,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -19445,7 +19307,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -19453,7 +19315,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -19461,7 +19323,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -19469,7 +19331,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -19477,7 +19339,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -19485,7 +19347,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -19493,7 +19355,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -19501,7 +19363,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -19509,7 +19371,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -19517,7 +19379,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>

</xml_diff>